<commit_message>
Added gtdb files and updated supp tables
</commit_message>
<xml_diff>
--- a/docs/Supplementary Tables.xlsx
+++ b/docs/Supplementary Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efrat\Documents\GitHub\microbiome-metabolome-curated-data\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796077A9-9340-4EFC-9700-A8A7368C73BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320AC4D8-D501-43C1-B96F-0FA8AF052C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C58E8523-33F6-4E0C-953F-5B6F4D40C8B0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="200">
   <si>
     <t>Dataset ID (1)</t>
   </si>
@@ -1211,7 +1211,7 @@
       <pane xSplit="1" ySplit="11" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="R20" sqref="R20"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1751,8 +1751,8 @@
       <c r="D19" s="12">
         <v>42</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>27</v>
+      <c r="E19" s="12">
+        <v>54</v>
       </c>
       <c r="F19" s="12">
         <v>42</v>

</xml_diff>

<commit_message>
16S datasets now based on GTDB taxonomy
</commit_message>
<xml_diff>
--- a/docs/Supplementary Tables.xlsx
+++ b/docs/Supplementary Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efrat\Documents\GitHub\microbiome-metabolome-curated-data\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320AC4D8-D501-43C1-B96F-0FA8AF052C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152BF305-E614-4FAF-B43A-363C84840C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C58E8523-33F6-4E0C-953F-5B6F4D40C8B0}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Table S2" sheetId="3" r:id="rId3"/>
     <sheet name="Table S3" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="198">
   <si>
     <t>Dataset ID (1)</t>
   </si>
@@ -349,9 +349,6 @@
     <t>Provided in data</t>
   </si>
   <si>
-    <t>NA (see comments)</t>
-  </si>
-  <si>
     <t>Longitudinal samples (over 6 months) from patients with Irritable Bowel Syndrome and controls.</t>
   </si>
   <si>
@@ -368,9 +365,6 @@
   </si>
   <si>
     <t>Infants over several time points during the 1st year of life, either breast-fed, formula-fed, or experimental formula fed.</t>
-  </si>
-  <si>
-    <t>We used only the samples from month 12 per infant, who also consumed complementary foods.</t>
   </si>
   <si>
     <t>68 (see comments)</t>
@@ -1168,31 +1162,31 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -1211,7 +1205,7 @@
       <pane xSplit="1" ySplit="11" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1237,7 +1231,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
@@ -1247,22 +1241,22 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
@@ -1297,7 +1291,7 @@
         <v>6</v>
       </c>
       <c r="Q10" s="25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="R10" s="25" t="s">
         <v>7</v>
@@ -1319,7 +1313,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>10</v>
@@ -1328,10 +1322,10 @@
         <v>11</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>12</v>
@@ -1351,10 +1345,10 @@
     </row>
     <row r="12" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="12">
         <v>127</v>
@@ -1369,7 +1363,7 @@
         <v>220</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>15</v>
@@ -1384,7 +1378,7 @@
         <v>17</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>18</v>
@@ -1402,15 +1396,15 @@
         <v>21</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C13" s="12">
         <v>56</v>
@@ -1425,7 +1419,7 @@
         <v>157</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>15</v>
@@ -1440,7 +1434,7 @@
         <v>27</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>23</v>
@@ -1460,10 +1454,10 @@
     </row>
     <row r="14" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C14" s="12">
         <v>89</v>
@@ -1508,21 +1502,21 @@
         <v>20</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B15" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>27</v>
@@ -1564,18 +1558,15 @@
         <v>35</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="R15" s="4" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C16" s="12">
         <v>26</v>
@@ -1590,7 +1581,7 @@
         <v>212</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>36</v>
@@ -1623,15 +1614,15 @@
         <v>39</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C17" s="12">
         <v>54</v>
@@ -1661,7 +1652,7 @@
         <v>42</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M17" s="4" t="s">
         <v>23</v>
@@ -1684,7 +1675,7 @@
     </row>
     <row r="18" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>45</v>
@@ -1702,10 +1693,10 @@
         <v>27</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>16</v>
@@ -1714,10 +1705,10 @@
         <v>22</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L18" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>23</v>
@@ -1726,7 +1717,7 @@
         <v>38</v>
       </c>
       <c r="O18" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="P18" s="4" t="s">
         <v>20</v>
@@ -1735,18 +1726,18 @@
         <v>46</v>
       </c>
       <c r="R18" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>103</v>
+        <v>130</v>
+      </c>
+      <c r="C19" s="12">
+        <v>54</v>
       </c>
       <c r="D19" s="12">
         <v>42</v>
@@ -1758,7 +1749,7 @@
         <v>42</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>15</v>
@@ -1791,7 +1782,7 @@
         <v>49</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="58" x14ac:dyDescent="0.35">
@@ -1799,7 +1790,7 @@
         <v>61</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C20" s="12">
         <v>102</v>
@@ -1844,15 +1835,15 @@
         <v>20</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C21" s="12">
         <v>24</v>
@@ -1867,7 +1858,7 @@
         <v>143</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>54</v>
@@ -1900,15 +1891,15 @@
         <v>58</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C22" s="4">
         <v>21</v>
@@ -1923,10 +1914,10 @@
         <v>23</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>27</v>
@@ -1935,7 +1926,7 @@
         <v>27</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="L22" s="4" t="s">
         <v>34</v>
@@ -1944,7 +1935,7 @@
         <v>18</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="O22" s="4" t="s">
         <v>20</v>
@@ -1953,15 +1944,15 @@
         <v>20</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C23" s="4">
         <v>8</v>
@@ -1985,13 +1976,13 @@
         <v>16</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L23" s="24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="M23" s="4" t="s">
         <v>23</v>
@@ -2006,15 +1997,15 @@
         <v>20</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C24" s="4">
         <v>21</v>
@@ -2038,28 +2029,28 @@
         <v>16</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M24" s="4" t="s">
         <v>23</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="P24" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2106,7 +2097,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -2116,12 +2107,12 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -2144,7 +2135,7 @@
       <c r="H8" s="27"/>
       <c r="I8" s="27"/>
       <c r="J8" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -2185,7 +2176,7 @@
         <v>74</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>75</v>
@@ -2197,7 +2188,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>77</v>
@@ -2229,7 +2220,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>77</v>
@@ -2261,10 +2252,10 @@
     </row>
     <row r="13" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>77</v>
@@ -2285,7 +2276,7 @@
         <v>77</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J13" s="7" t="s">
         <v>77</v>
@@ -2317,7 +2308,7 @@
         <v>82</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J14" s="7" t="s">
         <v>77</v>
@@ -2325,7 +2316,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>77</v>
@@ -2357,7 +2348,7 @@
     </row>
     <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>78</v>
@@ -2381,7 +2372,7 @@
         <v>84</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J16" s="7" t="s">
         <v>77</v>
@@ -2389,7 +2380,7 @@
     </row>
     <row r="17" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>78</v>
@@ -2413,7 +2404,7 @@
         <v>88</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J17" s="7" t="s">
         <v>77</v>
@@ -2421,7 +2412,7 @@
     </row>
     <row r="18" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>77</v>
@@ -2477,7 +2468,7 @@
         <v>90</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J19" s="7" t="s">
         <v>77</v>
@@ -2485,7 +2476,7 @@
     </row>
     <row r="20" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>77</v>
@@ -2512,12 +2503,12 @@
         <v>77</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>78</v>
@@ -2535,13 +2526,13 @@
         <v>79</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J21" s="7" t="s">
         <v>77</v>
@@ -2549,7 +2540,7 @@
     </row>
     <row r="22" spans="1:10" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>78</v>
@@ -2567,13 +2558,13 @@
         <v>78</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>84</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>77</v>
@@ -2581,7 +2572,7 @@
     </row>
     <row r="23" spans="1:10" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>78</v>
@@ -2599,13 +2590,13 @@
         <v>78</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H23" s="3">
         <v>275</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>77</v>
@@ -2648,7 +2639,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -2665,12 +2656,12 @@
         <v>93</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>99</v>
@@ -2687,7 +2678,7 @@
     </row>
     <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>100</v>
@@ -2704,10 +2695,10 @@
     </row>
     <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>96</v>
@@ -2738,7 +2729,7 @@
     </row>
     <row r="8" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>101</v>
@@ -2755,10 +2746,10 @@
     </row>
     <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>95</v>
@@ -2772,7 +2763,7 @@
     </row>
     <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>97</v>
@@ -2789,7 +2780,7 @@
     </row>
     <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>99</v>
@@ -2823,7 +2814,7 @@
     </row>
     <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>97</v>
@@ -2840,7 +2831,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>97</v>
@@ -2857,10 +2848,10 @@
     </row>
     <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>96</v>
@@ -2874,13 +2865,13 @@
     </row>
     <row r="16" spans="1:5" s="23" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D16" s="15">
         <v>453</v>

</xml_diff>

<commit_message>
Updated data organization logic
Mapping taxonomy to GTDB
</commit_message>
<xml_diff>
--- a/docs/Supplementary Tables.xlsx
+++ b/docs/Supplementary Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efrat\Documents\GitHub\microbiome-metabolome-curated-data\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152BF305-E614-4FAF-B43A-363C84840C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4085B739-06B1-4D5C-ACD7-71E58E727CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C58E8523-33F6-4E0C-953F-5B6F4D40C8B0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C58E8523-33F6-4E0C-953F-5B6F4D40C8B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Table of Contents" sheetId="1" r:id="rId1"/>
@@ -394,15 +394,9 @@
     <t>No, BURST-based species-level taxonomy was used instead</t>
   </si>
   <si>
-    <t>Raw 16S data was unavailable (processed data was used instead).</t>
-  </si>
-  <si>
     <t>No, QIIME-based genus-level taxonomy was used instead</t>
   </si>
   <si>
-    <t>OTU clustering and alignment to IMG/GG GreenGenes genomes (QIIME)</t>
-  </si>
-  <si>
     <t>Trained a NB classifier (QIIME2)</t>
   </si>
   <si>
@@ -632,13 +626,19 @@
   </si>
   <si>
     <t>Control subjects are shared with YACHIDA_CRC study (a column indicating which subjects exactly was added to the metadata)</t>
+  </si>
+  <si>
+    <t>Raw 16S data was unavailable (processed data was used instead, and taxonomy mapped to GTDB only when mapping was confident).</t>
+  </si>
+  <si>
+    <t>OTU clustering and alignment with QIIME1 (in original study). Mapping to GTDB where confident.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,13 +673,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -721,6 +714,21 @@
       <charset val="177"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -753,9 +761,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -785,26 +793,23 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -814,13 +819,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -833,6 +835,18 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1162,35 +1176,35 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="B3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="B4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="20"/>
+      <c r="A6" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1201,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57439337-C632-449F-95CC-9CA24940408D}">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="11" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="11" topLeftCell="J12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
       <selection pane="bottomRight" activeCell="R15" sqref="R15"/>
@@ -1231,75 +1245,75 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
-        <v>191</v>
-      </c>
-    </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
-        <v>192</v>
+      <c r="A5" s="12" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
-        <v>195</v>
+      <c r="A6" s="12" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26" t="s">
+      <c r="D10" s="24"/>
+      <c r="E10" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26" t="s">
+      <c r="F10" s="24"/>
+      <c r="G10" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26" t="s">
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="25" t="s">
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="Q10" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="R10" s="25" t="s">
+      <c r="Q10" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="R10" s="23" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="58" x14ac:dyDescent="0.35">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1313,7 +1327,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>10</v>
@@ -1322,10 +1336,10 @@
         <v>11</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>12</v>
@@ -1339,31 +1353,31 @@
       <c r="O11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
     </row>
     <row r="12" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B12" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="11">
         <v>127</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="11">
         <v>220</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="11">
         <v>127</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="11">
         <v>220</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>15</v>
@@ -1377,7 +1391,7 @@
       <c r="K12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="L12" s="11" t="s">
         <v>116</v>
       </c>
       <c r="M12" s="4" t="s">
@@ -1396,30 +1410,30 @@
         <v>21</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B13" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="11">
         <v>56</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="11">
         <v>157</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="11">
         <v>56</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="11">
         <v>157</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>15</v>
@@ -1433,7 +1447,7 @@
       <c r="K13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L13" s="12" t="s">
+      <c r="L13" s="11" t="s">
         <v>115</v>
       </c>
       <c r="M13" s="4" t="s">
@@ -1452,23 +1466,23 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B14" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="11">
         <v>89</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="11">
         <v>42</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="11">
         <v>89</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="11">
         <v>42</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -1486,7 +1500,7 @@
       <c r="K14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L14" s="12" t="s">
+      <c r="L14" s="11" t="s">
         <v>20</v>
       </c>
       <c r="M14" s="4" t="s">
@@ -1502,17 +1516,17 @@
         <v>20</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>118</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B15" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>108</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1542,7 +1556,7 @@
       <c r="K15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="L15" s="11" t="s">
         <v>35</v>
       </c>
       <c r="M15" s="4" t="s">
@@ -1558,30 +1572,30 @@
         <v>35</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B16" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="11">
         <v>26</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="11">
         <v>79</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="11">
         <v>72</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="11">
         <v>212</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>36</v>
@@ -1595,7 +1609,7 @@
       <c r="K16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L16" s="12" t="s">
+      <c r="L16" s="11" t="s">
         <v>37</v>
       </c>
       <c r="M16" s="4" t="s">
@@ -1614,26 +1628,26 @@
         <v>39</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B17" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="11">
         <v>54</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="11">
         <v>54</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="11" t="s">
         <v>27</v>
       </c>
       <c r="G17" s="3" t="s">
@@ -1651,7 +1665,7 @@
       <c r="K17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="L17" s="12" t="s">
+      <c r="L17" s="11" t="s">
         <v>112</v>
       </c>
       <c r="M17" s="4" t="s">
@@ -1660,7 +1674,7 @@
       <c r="N17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="O17" s="18" t="s">
+      <c r="O17" s="17" t="s">
         <v>34</v>
       </c>
       <c r="P17" s="4" t="s">
@@ -1675,28 +1689,28 @@
     </row>
     <row r="18" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B18" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="11">
         <v>83</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="11">
         <v>141</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="11" t="s">
         <v>27</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>16</v>
@@ -1705,9 +1719,9 @@
         <v>22</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="L18" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="L18" s="11" t="s">
         <v>113</v>
       </c>
       <c r="M18" s="4" t="s">
@@ -1716,7 +1730,7 @@
       <c r="N18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="O18" s="12" t="s">
+      <c r="O18" s="11" t="s">
         <v>114</v>
       </c>
       <c r="P18" s="4" t="s">
@@ -1731,25 +1745,25 @@
     </row>
     <row r="19" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C19" s="12">
+        <v>144</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" s="11">
         <v>54</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="11">
         <v>42</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="11">
         <v>54</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="11">
         <v>42</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>15</v>
@@ -1772,36 +1786,36 @@
       <c r="N19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O19" s="18" t="s">
+      <c r="O19" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="P19" s="18" t="s">
+      <c r="P19" s="17" t="s">
         <v>34</v>
       </c>
       <c r="Q19" s="4" t="s">
         <v>49</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="C20" s="12">
+      <c r="B20" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="11">
         <v>102</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="11">
         <v>138</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="11">
         <v>102</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="11">
         <v>138</v>
       </c>
       <c r="G20" s="3" t="s">
@@ -1835,30 +1849,30 @@
         <v>20</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="11">
         <v>24</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="11">
         <v>51</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="11">
         <v>70</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="11">
         <v>143</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>54</v>
@@ -1872,7 +1886,7 @@
       <c r="K21" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="L21" s="12" t="s">
+      <c r="L21" s="11" t="s">
         <v>56</v>
       </c>
       <c r="M21" s="4" t="s">
@@ -1891,15 +1905,15 @@
         <v>58</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C22" s="4">
         <v>21</v>
@@ -1914,10 +1928,10 @@
         <v>23</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>27</v>
@@ -1926,7 +1940,7 @@
         <v>27</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L22" s="4" t="s">
         <v>34</v>
@@ -1935,7 +1949,7 @@
         <v>18</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O22" s="4" t="s">
         <v>20</v>
@@ -1944,15 +1958,15 @@
         <v>20</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C23" s="4">
         <v>8</v>
@@ -1976,13 +1990,13 @@
         <v>16</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="L23" s="24" t="s">
-        <v>173</v>
+        <v>166</v>
+      </c>
+      <c r="L23" s="22" t="s">
+        <v>171</v>
       </c>
       <c r="M23" s="4" t="s">
         <v>23</v>
@@ -1990,22 +2004,22 @@
       <c r="N23" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="O23" s="18" t="s">
+      <c r="O23" s="17" t="s">
         <v>34</v>
       </c>
       <c r="P23" s="4" t="s">
         <v>20</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C24" s="4">
         <v>21</v>
@@ -2029,28 +2043,28 @@
         <v>16</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M24" s="4" t="s">
         <v>23</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="P24" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2077,11 +2091,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6614462A-48C8-42E0-BE6C-65302361CC63}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
+      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2097,72 +2111,72 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
-        <v>127</v>
+      <c r="A4" s="13" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
-        <v>122</v>
+      <c r="A5" s="13" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
       <c r="J8" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="27"/>
-      <c r="B9" s="28" t="s">
+      <c r="A9" s="25"/>
+      <c r="B9" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28" t="s">
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="22" t="s">
+      <c r="H9" s="26"/>
+      <c r="I9" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="24" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="10" t="s">
         <v>71</v>
       </c>
@@ -2176,19 +2190,19 @@
         <v>74</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="J10" s="26"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>77</v>
@@ -2211,7 +2225,7 @@
       <c r="H11" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="29" t="s">
         <v>77</v>
       </c>
       <c r="J11" s="7" t="s">
@@ -2220,7 +2234,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>77</v>
@@ -2243,7 +2257,7 @@
       <c r="H12" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="29" t="s">
         <v>77</v>
       </c>
       <c r="J12" s="7" t="s">
@@ -2252,10 +2266,10 @@
     </row>
     <row r="13" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>77</v>
@@ -2275,8 +2289,8 @@
       <c r="H13" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="I13" s="9" t="s">
-        <v>120</v>
+      <c r="I13" s="30" t="s">
+        <v>197</v>
       </c>
       <c r="J13" s="7" t="s">
         <v>77</v>
@@ -2307,8 +2321,8 @@
       <c r="H14" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="I14" s="7" t="s">
-        <v>121</v>
+      <c r="I14" s="29" t="s">
+        <v>119</v>
       </c>
       <c r="J14" s="7" t="s">
         <v>77</v>
@@ -2316,7 +2330,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>77</v>
@@ -2339,7 +2353,7 @@
       <c r="H15" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="29" t="s">
         <v>77</v>
       </c>
       <c r="J15" s="7" t="s">
@@ -2348,7 +2362,7 @@
     </row>
     <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>78</v>
@@ -2371,8 +2385,8 @@
       <c r="H16" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="I16" s="7" t="s">
-        <v>121</v>
+      <c r="I16" s="29" t="s">
+        <v>119</v>
       </c>
       <c r="J16" s="7" t="s">
         <v>77</v>
@@ -2380,7 +2394,7 @@
     </row>
     <row r="17" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>78</v>
@@ -2403,8 +2417,8 @@
       <c r="H17" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="I17" s="7" t="s">
-        <v>121</v>
+      <c r="I17" s="29" t="s">
+        <v>119</v>
       </c>
       <c r="J17" s="7" t="s">
         <v>77</v>
@@ -2412,7 +2426,7 @@
     </row>
     <row r="18" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>77</v>
@@ -2435,7 +2449,7 @@
       <c r="H18" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I18" s="29" t="s">
         <v>77</v>
       </c>
       <c r="J18" s="7" t="s">
@@ -2467,8 +2481,8 @@
       <c r="H19" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="I19" s="7" t="s">
-        <v>121</v>
+      <c r="I19" s="29" t="s">
+        <v>119</v>
       </c>
       <c r="J19" s="7" t="s">
         <v>77</v>
@@ -2476,7 +2490,7 @@
     </row>
     <row r="20" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>77</v>
@@ -2499,7 +2513,7 @@
       <c r="H20" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="I20" s="7" t="s">
+      <c r="I20" s="29" t="s">
         <v>77</v>
       </c>
       <c r="J20" s="9" t="s">
@@ -2508,7 +2522,7 @@
     </row>
     <row r="21" spans="1:10" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>78</v>
@@ -2526,13 +2540,13 @@
         <v>79</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>121</v>
+        <v>165</v>
+      </c>
+      <c r="I21" s="29" t="s">
+        <v>119</v>
       </c>
       <c r="J21" s="7" t="s">
         <v>77</v>
@@ -2540,7 +2554,7 @@
     </row>
     <row r="22" spans="1:10" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>78</v>
@@ -2558,13 +2572,13 @@
         <v>78</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="I22" s="7" t="s">
-        <v>121</v>
+      <c r="I22" s="29" t="s">
+        <v>119</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>77</v>
@@ -2572,7 +2586,7 @@
     </row>
     <row r="23" spans="1:10" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>78</v>
@@ -2590,13 +2604,13 @@
         <v>78</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H23" s="3">
         <v>275</v>
       </c>
-      <c r="I23" s="7" t="s">
-        <v>121</v>
+      <c r="I23" s="29" t="s">
+        <v>119</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>77</v>
@@ -2639,7 +2653,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -2656,57 +2670,57 @@
         <v>93</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="B4" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
         <v>450</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="14">
         <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B5" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>8848</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="C6" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>530</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>352</v>
       </c>
     </row>
@@ -2714,84 +2728,84 @@
       <c r="A7" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>120</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B8" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <v>81867</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <v>455</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="C9" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>4626</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B10" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="14">
         <v>489</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="14">
         <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="B11" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="15">
         <v>524</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="14">
         <v>462</v>
       </c>
     </row>
@@ -2799,84 +2813,84 @@
       <c r="A12" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="15">
         <v>462</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="14">
         <v>358</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="B13" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B13" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="14">
         <v>43</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="14">
         <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B14" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="14">
         <v>61</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="14">
         <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="C15" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="C15" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="14">
         <v>184</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="14">
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="23" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="D16" s="15">
+    <row r="16" spans="1:5" s="21" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="D16" s="14">
         <v>453</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="14">
         <v>198</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data updated (shotgun data - temporary versions only)
</commit_message>
<xml_diff>
--- a/docs/Supplementary Tables.xlsx
+++ b/docs/Supplementary Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efrat\Documents\GitHub\microbiome-metabolome-curated-data\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0359DE25-E4A5-4A05-9424-548FBDB60D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FB04B5-2F5C-408D-925C-8984DA83A87E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C58E8523-33F6-4E0C-953F-5B6F4D40C8B0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{C58E8523-33F6-4E0C-953F-5B6F4D40C8B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Table of Contents" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="194">
   <si>
     <t>Dataset ID (1)</t>
   </si>
@@ -331,9 +331,6 @@
     <t>Metabolites were identified by name only.</t>
   </si>
   <si>
-    <t>Cases were excluded as there were less than 40.</t>
-  </si>
-  <si>
     <t>Metabolites were identified by name and most also had KEGG ID's.</t>
   </si>
   <si>
@@ -349,9 +346,6 @@
     <t>Longitudinal samples (over 6 months) from patients with Irritable Bowel Syndrome and controls.</t>
   </si>
   <si>
-    <t>Inflammatory bowel disease patients and their first degree relatives of patients with IBD.</t>
-  </si>
-  <si>
     <t>Patients who underwent colonoscopy, with findings from normal to stage 4 colorectal cancer.</t>
   </si>
   <si>
@@ -364,9 +358,6 @@
     <t>Infants over several time points during the 1st year of life, either breast-fed, formula-fed, or experimental formula fed.</t>
   </si>
   <si>
-    <t>68 (see comments)</t>
-  </si>
-  <si>
     <t>HMP2 (integrative HMP) cohort: Inflammatory bowel disease patients who were profiled several times over the course of a year.</t>
   </si>
   <si>
@@ -517,9 +508,6 @@
     <t>16S V2-V3</t>
   </si>
   <si>
-    <t>FLX-Titanium (454)</t>
-  </si>
-  <si>
     <t>41K</t>
   </si>
   <si>
@@ -538,9 +526,6 @@
     <t>46K</t>
   </si>
   <si>
-    <t>Children at risk for T1D, from the DIABIMMUNE cohort</t>
-  </si>
-  <si>
     <t>2 X 175</t>
   </si>
   <si>
@@ -629,6 +614,12 @@
   </si>
   <si>
     <t>TBC</t>
+  </si>
+  <si>
+    <t>Inflammatory bowel disease patients and their first degree (healthy) relatives.</t>
+  </si>
+  <si>
+    <t>Longitudinal samples from children at risk for T1D (DIABIMMUNE cohort).</t>
   </si>
 </sst>
 </file>
@@ -825,18 +816,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -849,6 +828,18 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1170,7 +1161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{847F1507-5CF3-4099-A5F0-0BA103DB973E}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1180,31 +1171,31 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -1220,10 +1211,10 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="11" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="11" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="Q14" sqref="Q14"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1249,7 +1240,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
@@ -1259,65 +1250,65 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25" t="s">
+      <c r="D10" s="30"/>
+      <c r="E10" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25" t="s">
+      <c r="F10" s="30"/>
+      <c r="G10" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25" t="s">
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="24" t="s">
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="Q10" s="24" t="s">
-        <v>170</v>
-      </c>
-      <c r="R10" s="24" t="s">
+      <c r="Q10" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="R10" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="58" x14ac:dyDescent="0.35">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1331,7 +1322,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>10</v>
@@ -1340,10 +1331,10 @@
         <v>11</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>12</v>
@@ -1357,16 +1348,16 @@
       <c r="O11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="29"/>
     </row>
     <row r="12" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C12" s="11">
         <v>127</v>
@@ -1381,7 +1372,7 @@
         <v>220</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>15</v>
@@ -1396,7 +1387,7 @@
         <v>17</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>18</v>
@@ -1414,15 +1405,15 @@
         <v>21</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C13" s="11">
         <v>56</v>
@@ -1437,7 +1428,7 @@
         <v>157</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>15</v>
@@ -1452,7 +1443,7 @@
         <v>27</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>23</v>
@@ -1472,10 +1463,10 @@
     </row>
     <row r="14" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C14" s="11">
         <v>89</v>
@@ -1520,27 +1511,27 @@
         <v>20</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
+      </c>
+      <c r="C15" s="4">
+        <v>80</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="4">
-        <v>68</v>
+        <v>277</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>27</v>
@@ -1576,15 +1567,15 @@
         <v>35</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C16" s="11">
         <v>26</v>
@@ -1593,13 +1584,13 @@
         <v>79</v>
       </c>
       <c r="E16" s="11">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="F16" s="11">
-        <v>212</v>
+        <v>286</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>36</v>
@@ -1632,27 +1623,27 @@
         <v>39</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="58" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>103</v>
+        <v>192</v>
       </c>
       <c r="C17" s="11">
         <v>54</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>27</v>
+      <c r="D17" s="11">
+        <v>36</v>
       </c>
       <c r="E17" s="11">
         <v>54</v>
       </c>
-      <c r="F17" s="11" t="s">
-        <v>27</v>
+      <c r="F17" s="11">
+        <v>36</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>30</v>
@@ -1670,7 +1661,7 @@
         <v>42</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="M17" s="4" t="s">
         <v>23</v>
@@ -1687,13 +1678,10 @@
       <c r="Q17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="R17" s="4" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="18" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B18" s="17" t="s">
         <v>45</v>
@@ -1705,16 +1693,16 @@
         <v>27</v>
       </c>
       <c r="E18" s="11">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>27</v>
       </c>
       <c r="G18" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>16</v>
@@ -1723,10 +1711,10 @@
         <v>22</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>23</v>
@@ -1735,7 +1723,7 @@
         <v>38</v>
       </c>
       <c r="O18" s="11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="P18" s="4" t="s">
         <v>20</v>
@@ -1744,15 +1732,15 @@
         <v>46</v>
       </c>
       <c r="R18" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C19" s="11">
         <v>54</v>
@@ -1767,7 +1755,7 @@
         <v>42</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>15</v>
@@ -1800,7 +1788,7 @@
         <v>49</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="58" x14ac:dyDescent="0.35">
@@ -1808,7 +1796,7 @@
         <v>61</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C20" s="11">
         <v>102</v>
@@ -1853,15 +1841,15 @@
         <v>20</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" s="11">
         <v>24</v>
@@ -1870,13 +1858,13 @@
         <v>51</v>
       </c>
       <c r="E21" s="11">
-        <v>70</v>
+        <v>142</v>
       </c>
       <c r="F21" s="11">
-        <v>143</v>
+        <v>313</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>54</v>
@@ -1909,15 +1897,15 @@
         <v>58</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>156</v>
       </c>
       <c r="C22" s="4">
         <v>21</v>
@@ -1932,10 +1920,10 @@
         <v>23</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
+      </c>
+      <c r="H22" s="3">
+        <v>454</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>27</v>
@@ -1944,7 +1932,7 @@
         <v>27</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L22" s="4" t="s">
         <v>34</v>
@@ -1953,7 +1941,7 @@
         <v>18</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="O22" s="4" t="s">
         <v>20</v>
@@ -1962,15 +1950,15 @@
         <v>20</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="C23" s="4">
         <v>8</v>
@@ -1994,13 +1982,13 @@
         <v>16</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="K23" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="L23" s="22" t="s">
         <v>163</v>
-      </c>
-      <c r="L23" s="22" t="s">
-        <v>168</v>
       </c>
       <c r="M23" s="4" t="s">
         <v>23</v>
@@ -2015,15 +2003,15 @@
         <v>20</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C24" s="4">
         <v>21</v>
@@ -2047,28 +2035,28 @@
         <v>16</v>
       </c>
       <c r="J24" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="L24" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>179</v>
       </c>
       <c r="M24" s="4" t="s">
         <v>23</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="P24" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2095,11 +2083,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6614462A-48C8-42E0-BE6C-65302361CC63}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="N19" sqref="N19"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2109,13 +2097,13 @@
     <col min="3" max="6" width="17.36328125" customWidth="1"/>
     <col min="7" max="7" width="24.90625" customWidth="1"/>
     <col min="8" max="8" width="10.6328125" customWidth="1"/>
-    <col min="9" max="9" width="34.26953125" style="28" customWidth="1"/>
+    <col min="9" max="9" width="34.26953125" style="24" customWidth="1"/>
     <col min="10" max="10" width="26.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
@@ -2125,12 +2113,12 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -2139,52 +2127,52 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27" t="s">
+      <c r="A9" s="32"/>
+      <c r="B9" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27" t="s">
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="H9" s="27"/>
-      <c r="I9" s="29" t="s">
+      <c r="H9" s="31"/>
+      <c r="I9" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="31" t="s">
         <v>66</v>
       </c>
       <c r="K9" s="33"/>
       <c r="L9" s="33"/>
     </row>
     <row r="10" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="10" t="s">
         <v>70</v>
       </c>
@@ -2198,25 +2186,25 @@
         <v>73</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="I10" s="30" t="s">
+      <c r="I10" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="J10" s="27"/>
+      <c r="J10" s="31"/>
       <c r="K10" s="23" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="L10" s="23" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>76</v>
@@ -2248,7 +2236,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>76</v>
@@ -2280,10 +2268,10 @@
     </row>
     <row r="13" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>76</v>
@@ -2303,8 +2291,8 @@
       <c r="H13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="I13" s="31" t="s">
-        <v>194</v>
+      <c r="I13" s="27" t="s">
+        <v>189</v>
       </c>
       <c r="J13" s="7" t="s">
         <v>76</v>
@@ -2342,7 +2330,7 @@
         <v>81</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="J14" s="7" t="s">
         <v>76</v>
@@ -2356,7 +2344,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>76</v>
@@ -2388,7 +2376,7 @@
     </row>
     <row r="16" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>77</v>
@@ -2412,7 +2400,7 @@
         <v>83</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="J16" s="7" t="s">
         <v>76</v>
@@ -2426,7 +2414,7 @@
     </row>
     <row r="17" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>77</v>
@@ -2450,7 +2438,7 @@
         <v>87</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="J17" s="7" t="s">
         <v>76</v>
@@ -2464,7 +2452,7 @@
     </row>
     <row r="18" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>76</v>
@@ -2520,7 +2508,7 @@
         <v>89</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="J19" s="7" t="s">
         <v>76</v>
@@ -2534,7 +2522,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>76</v>
@@ -2566,7 +2554,7 @@
     </row>
     <row r="21" spans="1:12" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>77</v>
@@ -2584,13 +2572,13 @@
         <v>78</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="J21" s="7" t="s">
         <v>76</v>
@@ -2604,7 +2592,7 @@
     </row>
     <row r="22" spans="1:12" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>77</v>
@@ -2622,13 +2610,13 @@
         <v>77</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>83</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>76</v>
@@ -2642,7 +2630,7 @@
     </row>
     <row r="23" spans="1:12" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>77</v>
@@ -2660,13 +2648,13 @@
         <v>77</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="H23" s="3">
         <v>275</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>76</v>
@@ -2679,7 +2667,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="I24" s="32"/>
+      <c r="I24" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2719,7 +2707,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -2736,15 +2724,15 @@
         <v>92</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>93</v>
@@ -2758,10 +2746,10 @@
     </row>
     <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>94</v>
@@ -2775,10 +2763,10 @@
     </row>
     <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>95</v>
@@ -2809,13 +2797,13 @@
     </row>
     <row r="8" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B8" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>100</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>101</v>
       </c>
       <c r="D8" s="14">
         <v>81867</v>
@@ -2824,12 +2812,12 @@
         <v>455</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>94</v>
@@ -2843,7 +2831,7 @@
     </row>
     <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>96</v>
@@ -2860,10 +2848,10 @@
     </row>
     <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>93</v>
@@ -2894,7 +2882,7 @@
     </row>
     <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>96</v>
@@ -2911,7 +2899,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>96</v>
@@ -2928,10 +2916,10 @@
     </row>
     <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>95</v>
@@ -2945,13 +2933,13 @@
     </row>
     <row r="16" spans="1:5" s="21" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D16" s="14">
         <v>453</v>

</xml_diff>

<commit_message>
New dataset and misc. updates
</commit_message>
<xml_diff>
--- a/docs/Supplementary Tables.xlsx
+++ b/docs/Supplementary Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efrat\Documents\GitHub\microbiome-metabolome-curated-data\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6437C7-3190-4FA3-AF0A-49DA7C24CE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12930751-99FC-411B-A86D-CADD23B9004C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="735" windowWidth="29040" windowHeight="15720" xr2:uid="{C58E8523-33F6-4E0C-953F-5B6F4D40C8B0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{C58E8523-33F6-4E0C-953F-5B6F4D40C8B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Table of Contents" sheetId="1" r:id="rId1"/>
@@ -834,6 +834,9 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -848,9 +851,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1170,7 +1170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{847F1507-5CF3-4099-A5F0-0BA103DB973E}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1219,11 +1219,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57439337-C632-449F-95CC-9CA24940408D}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="10" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="C24:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1272,45 +1272,45 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30" t="s">
+      <c r="D9" s="31"/>
+      <c r="E9" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30" t="s">
+      <c r="F9" s="31"/>
+      <c r="G9" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30" t="s">
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="29" t="s">
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="P9" s="29" t="s">
+      <c r="P9" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="Q9" s="29" t="s">
+      <c r="Q9" s="30" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="29"/>
-      <c r="B10" s="29"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1347,9 +1347,9 @@
       <c r="N10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
     </row>
     <row r="11" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
@@ -1663,7 +1663,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="58" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>130</v>
       </c>
@@ -2147,60 +2147,60 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="29" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="32"/>
-      <c r="B10" s="31" t="s">
+      <c r="A10" s="33"/>
+      <c r="B10" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31" t="s">
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="31"/>
+      <c r="H10" s="32"/>
       <c r="I10" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="J10" s="31" t="s">
+      <c r="J10" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="K10" s="33" t="s">
+      <c r="K10" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
       <c r="N10" s="24" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="32"/>
-      <c r="B11" s="31"/>
+    <row r="11" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="33"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="10" t="s">
         <v>58</v>
       </c>
@@ -2222,7 +2222,7 @@
       <c r="I11" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="J11" s="31"/>
+      <c r="J11" s="32"/>
       <c r="K11" s="25" t="s">
         <v>176</v>
       </c>
@@ -2276,7 +2276,7 @@
       <c r="M12" s="27">
         <v>15186345.503253795</v>
       </c>
-      <c r="N12" s="34" t="s">
+      <c r="N12" s="29" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2320,7 +2320,7 @@
       <c r="M13" s="27">
         <v>14336757.303370787</v>
       </c>
-      <c r="N13" s="34" t="s">
+      <c r="N13" s="29" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2452,7 +2452,7 @@
       <c r="M16" s="27">
         <v>10817935.358227849</v>
       </c>
-      <c r="N16" s="34" t="s">
+      <c r="N16" s="29" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2584,7 +2584,7 @@
       <c r="M19" s="27">
         <v>16014616.402515722</v>
       </c>
-      <c r="N19" s="34" t="s">
+      <c r="N19" s="29" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2672,7 +2672,7 @@
       <c r="M21" s="27">
         <v>1164200.9822485207</v>
       </c>
-      <c r="N21" s="34" t="s">
+      <c r="N21" s="29" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2848,20 +2848,20 @@
       <c r="M25" s="27">
         <v>37378334.239726029</v>
       </c>
-      <c r="N25" s="34" t="s">
+      <c r="N25" s="29" t="s">
         <v>191</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="J9:N9"/>
     <mergeCell ref="J10:J11"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="G10:H10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="J9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId1"/>
@@ -2995,7 +2995,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>132</v>
       </c>

</xml_diff>